<commit_message>
push version 1.1.2 - - New vignettes - Added Creatine-phosphokinase to the data - Minor bug-fixes
</commit_message>
<xml_diff>
--- a/data-raw/Copy of analytes_complete_ref_unit_SKa.xlsx
+++ b/data-raw/Copy of analytes_complete_ref_unit_SKa.xlsx
@@ -1,13 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18730"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\r_projects\grintar\data-raw\D016\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\r_projects\citrulliner2\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E86A9140-E8F3-48CD-A429-4B5D78544387}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15530" windowHeight="6470" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -399,9 +400,6 @@
     <t>cortisol</t>
   </si>
   <si>
-    <t>creatinekinase</t>
-  </si>
-  <si>
     <t>creatinine</t>
   </si>
   <si>
@@ -823,6 +821,9 @@
   </si>
   <si>
     <t>FALSE</t>
+  </si>
+  <si>
+    <t>creatine-phosphokinase</t>
   </si>
 </sst>
 </file>
@@ -1196,8 +1197,8 @@
   <dimension ref="A1:N86"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A72" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B87" sqref="B87"/>
+      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.36328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1210,16 +1211,16 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>264</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>265</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>1</v>
@@ -1257,7 +1258,7 @@
         <v>11</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C2" t="s">
         <v>94</v>
@@ -1272,28 +1273,28 @@
         <v>#N/A</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.35">
@@ -1301,10 +1302,10 @@
         <v>12</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>95</v>
@@ -1316,28 +1317,28 @@
         <v>45</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.35">
@@ -1345,10 +1346,10 @@
         <v>13</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C4" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>117</v>
@@ -1360,28 +1361,28 @@
         <v>52</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.35">
@@ -1389,7 +1390,7 @@
         <v>14</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C5" t="s">
         <v>96</v>
@@ -1404,28 +1405,28 @@
         <v>#N/A</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.35">
@@ -1433,10 +1434,10 @@
         <v>15</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C6" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>97</v>
@@ -1448,28 +1449,28 @@
         <v>35</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.35">
@@ -1477,7 +1478,7 @@
         <v>16</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C7" t="s">
         <v>98</v>
@@ -1492,28 +1493,28 @@
         <v>#N/A</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.35">
@@ -1521,7 +1522,7 @@
         <v>17</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C8" t="s">
         <v>99</v>
@@ -1536,28 +1537,28 @@
         <v>#N/A</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.35">
@@ -1565,10 +1566,10 @@
         <v>18</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C9" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>121</v>
@@ -1580,28 +1581,28 @@
         <v>0.2</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.35">
@@ -1609,10 +1610,10 @@
         <v>19</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C10" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>122</v>
@@ -1624,26 +1625,26 @@
         <v>29</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="J10"/>
       <c r="K10" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.35">
@@ -1651,10 +1652,10 @@
         <v>20</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C11" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>123</v>
@@ -1666,25 +1667,25 @@
         <v>3</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.35">
@@ -1692,10 +1693,10 @@
         <v>21</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C12" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>100</v>
@@ -1707,25 +1708,25 @@
         <v>107</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.35">
@@ -1733,7 +1734,7 @@
         <v>22</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C13" t="s">
         <v>101</v>
@@ -1748,25 +1749,25 @@
         <v>#N/A</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="N13" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.35">
@@ -1774,10 +1775,10 @@
         <v>23</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C14" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>125</v>
@@ -1789,25 +1790,25 @@
         <v>0.64</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="M14" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="N14" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.35">
@@ -1815,13 +1816,13 @@
         <v>24</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C15" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>126</v>
+        <v>267</v>
       </c>
       <c r="E15" s="1">
         <v>0</v>
@@ -1830,25 +1831,25 @@
         <v>171</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="M15" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="N15" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.35">
@@ -1856,13 +1857,13 @@
         <v>25</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C16" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E16" s="1">
         <v>59</v>
@@ -1871,25 +1872,25 @@
         <v>104</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="L16" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="M16" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="N16" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.35">
@@ -1897,10 +1898,10 @@
         <v>26</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E17" s="1">
         <v>0.1</v>
@@ -1909,25 +1910,25 @@
         <v>0.5</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="L17" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="M17" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="N17" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.35">
@@ -1935,13 +1936,13 @@
         <v>27</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C18" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E18" s="1">
         <v>4.3</v>
@@ -1950,25 +1951,25 @@
         <v>6</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="L18" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="M18" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="N18" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.35">
@@ -1976,13 +1977,13 @@
         <v>28</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C19" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E19" s="1">
         <v>0</v>
@@ -1991,26 +1992,26 @@
         <v>55</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="J19"/>
       <c r="K19" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="L19" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="M19" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="N19" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.35">
@@ -2018,10 +2019,10 @@
         <v>29</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E20" s="1" t="e">
         <v>#N/A</v>
@@ -2033,22 +2034,22 @@
         <v>#N/A</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="L20" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="M20" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="N20" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.35">
@@ -2056,13 +2057,13 @@
         <v>30</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C21" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E21" s="1">
         <v>4</v>
@@ -2071,25 +2072,25 @@
         <v>6</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="L21" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="M21" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="N21" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.35">
@@ -2097,13 +2098,13 @@
         <v>31</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C22" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E22" s="1" t="e">
         <v>#N/A</v>
@@ -2112,26 +2113,26 @@
         <v>#N/A</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="J22"/>
       <c r="K22" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="L22" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="M22" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="N22" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.35">
@@ -2139,13 +2140,13 @@
         <v>32</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C23" t="s">
         <v>102</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E23" s="1" t="e">
         <v>#N/A</v>
@@ -2154,25 +2155,25 @@
         <v>#N/A</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="L23" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="M23" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="N23" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.35">
@@ -2180,13 +2181,13 @@
         <v>33</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C24" t="s">
         <v>103</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E24" s="1" t="e">
         <v>#N/A</v>
@@ -2195,28 +2196,28 @@
         <v>#N/A</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="L24" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="M24" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="N24" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.35">
@@ -2224,13 +2225,13 @@
         <v>34</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C25" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E25" s="1">
         <v>0.4</v>
@@ -2239,28 +2240,28 @@
         <v>0.5</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="L25" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="M25" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="N25" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.35">
@@ -2268,13 +2269,13 @@
         <v>35</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C26" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E26" s="1">
         <v>8.5</v>
@@ -2283,28 +2284,28 @@
         <v>11</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="L26" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="M26" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="N26" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.35">
@@ -2312,13 +2313,13 @@
         <v>36</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C27" t="s">
         <v>104</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E27" s="1" t="e">
         <v>#N/A</v>
@@ -2327,28 +2328,28 @@
         <v>#N/A</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="L27" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="M27" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="N27" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.35">
@@ -2356,13 +2357,13 @@
         <v>37</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C28" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E28" s="1">
         <v>2.6</v>
@@ -2371,28 +2372,28 @@
         <v>24.9</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="L28" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="M28" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="N28" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.35">
@@ -2400,13 +2401,13 @@
         <v>38</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C29" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E29" s="1">
         <v>20</v>
@@ -2415,25 +2416,25 @@
         <v>5000</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="K29" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="L29" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="M29" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="N29" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.35">
@@ -2441,13 +2442,13 @@
         <v>39</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C30" t="s">
         <v>105</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E30" s="1" t="e">
         <v>#N/A</v>
@@ -2456,25 +2457,25 @@
         <v>#N/A</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="K30" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="L30" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="M30" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="N30" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.35">
@@ -2482,13 +2483,13 @@
         <v>40</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C31" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E31" s="1">
         <v>0</v>
@@ -2497,25 +2498,25 @@
         <v>248</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="K31" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="L31" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="M31" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="N31" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.35">
@@ -2523,13 +2524,13 @@
         <v>41</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C32" t="s">
         <v>106</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E32" s="1" t="e">
         <v>#N/A</v>
@@ -2538,25 +2539,25 @@
         <v>#N/A</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="K32" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="L32" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="M32" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="N32" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.35">
@@ -2564,13 +2565,13 @@
         <v>42</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C33" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E33" s="1">
         <v>4</v>
@@ -2579,25 +2580,25 @@
         <v>10</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="K33" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="L33" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="M33" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="N33" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.35">
@@ -2605,13 +2606,13 @@
         <v>43</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C34" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E34" s="1">
         <v>1</v>
@@ -2620,25 +2621,25 @@
         <v>3.5</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="K34" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="L34" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="M34" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="N34" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.35">
@@ -2646,13 +2647,13 @@
         <v>44</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C35" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E35" s="1">
         <v>1</v>
@@ -2661,25 +2662,25 @@
         <v>3.5</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="K35" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="L35" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="M35" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="N35" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.35">
@@ -2687,13 +2688,13 @@
         <v>45</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C36" t="s">
         <v>107</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E36" s="1" t="e">
         <v>#N/A</v>
@@ -2702,25 +2703,25 @@
         <v>#N/A</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="K36" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="L36" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="M36" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="N36" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.35">
@@ -2728,13 +2729,13 @@
         <v>46</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C37" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E37" s="1">
         <v>19</v>
@@ -2743,25 +2744,25 @@
         <v>22</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="K37" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="L37" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="M37" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="N37" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.35">
@@ -2769,13 +2770,13 @@
         <v>47</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C38" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E38" s="1">
         <v>80</v>
@@ -2784,25 +2785,25 @@
         <v>100</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="K38" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="L38" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="M38" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="N38" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.35">
@@ -2810,13 +2811,13 @@
         <v>48</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C39" t="s">
         <v>108</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E39" s="1" t="e">
         <v>#N/A</v>
@@ -2825,25 +2826,25 @@
         <v>#N/A</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="K39" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="L39" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="M39" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="N39" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.35">
@@ -2851,13 +2852,13 @@
         <v>49</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C40" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E40" s="1">
         <v>0.1</v>
@@ -2866,25 +2867,25 @@
         <v>1</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="K40" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="L40" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="M40" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="N40" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.35">
@@ -2892,13 +2893,13 @@
         <v>50</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C41" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E41" s="1">
         <v>1.5</v>
@@ -2907,25 +2908,25 @@
         <v>7.5</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="K41" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="L41" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="M41" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="N41" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.35">
@@ -2933,13 +2934,13 @@
         <v>51</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C42" t="s">
         <v>109</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E42" s="1" t="e">
         <v>#N/A</v>
@@ -2948,25 +2949,25 @@
         <v>#N/A</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I42" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="K42" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="L42" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="M42" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="N42" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.35">
@@ -2974,13 +2975,13 @@
         <v>52</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C43" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E43" s="1">
         <v>3.5</v>
@@ -2989,25 +2990,25 @@
         <v>5.3</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="I43" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="K43" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="L43" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="M43" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="N43" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.35">
@@ -3015,13 +3016,13 @@
         <v>53</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C44" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E44" s="1" t="e">
         <v>#N/A</v>
@@ -3033,22 +3034,22 @@
         <v>#N/A</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="I44" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="K44" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="L44" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="M44" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="N44" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.35">
@@ -3056,13 +3057,13 @@
         <v>54</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C45" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E45" s="1">
         <v>25</v>
@@ -3071,28 +3072,28 @@
         <v>120</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="I45" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="J45" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="K45" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="L45" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="M45" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="N45" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.35">
@@ -3100,13 +3101,13 @@
         <v>55</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C46" t="s">
         <v>110</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E46" s="1" t="e">
         <v>#N/A</v>
@@ -3115,28 +3116,28 @@
         <v>#N/A</v>
       </c>
       <c r="G46" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I46" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="J46" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="K46" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="L46" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="M46" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="N46" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.35">
@@ -3144,13 +3145,13 @@
         <v>56</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C47" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E47" s="1">
         <v>135</v>
@@ -3159,22 +3160,22 @@
         <v>145</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="K47" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="L47" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="M47" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="N47" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.35">
@@ -3182,13 +3183,13 @@
         <v>57</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C48" t="s">
         <v>111</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E48" s="1" t="e">
         <v>#N/A</v>
@@ -3197,28 +3198,28 @@
         <v>#N/A</v>
       </c>
       <c r="G48" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="H48" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I48" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="J48" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="K48" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="L48" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="M48" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="N48" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.35">
@@ -3226,13 +3227,13 @@
         <v>58</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C49" t="s">
         <v>112</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E49" s="1" t="e">
         <v>#N/A</v>
@@ -3241,25 +3242,25 @@
         <v>#N/A</v>
       </c>
       <c r="G49" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="H49" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I49" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="K49" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="L49" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="M49" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="N49" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.35">
@@ -3267,13 +3268,13 @@
         <v>59</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C50" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E50" s="1">
         <v>150</v>
@@ -3282,25 +3283,25 @@
         <v>400</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H50" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="J50" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="K50" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="L50" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="M50" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="N50" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.35">
@@ -3308,13 +3309,13 @@
         <v>60</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C51" t="s">
         <v>113</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E51" s="1" t="e">
         <v>#N/A</v>
@@ -3323,25 +3324,25 @@
         <v>#N/A</v>
       </c>
       <c r="G51" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="H51" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="J51" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="K51" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="L51" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="M51" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="N51" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.35">
@@ -3349,13 +3350,13 @@
         <v>61</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C52" t="s">
         <v>114</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E52" s="1" t="e">
         <v>#N/A</v>
@@ -3364,25 +3365,25 @@
         <v>#N/A</v>
       </c>
       <c r="G52" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="H52" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="J52" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="K52" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="L52" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="M52" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="N52" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.35">
@@ -3390,13 +3391,13 @@
         <v>62</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C53" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E53" s="1">
         <v>2.5</v>
@@ -3405,28 +3406,28 @@
         <v>6.4</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="H53" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="I53" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="J53" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="K53" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="L53" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="M53" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="N53" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.35">
@@ -3434,13 +3435,13 @@
         <v>63</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C54" t="s">
         <v>115</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E54" s="1" t="e">
         <v>#N/A</v>
@@ -3449,28 +3450,28 @@
         <v>#N/A</v>
       </c>
       <c r="G54" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="H54" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I54" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="J54" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="K54" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="L54" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="M54" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="N54" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="55" spans="1:14" x14ac:dyDescent="0.35">
@@ -3478,13 +3479,13 @@
         <v>64</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C55" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E55" s="1" t="e">
         <v>#N/A</v>
@@ -3499,19 +3500,19 @@
         <v>#N/A</v>
       </c>
       <c r="J55" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="K55" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="L55" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="M55" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="N55" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.35">
@@ -3519,13 +3520,13 @@
         <v>65</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C56" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E56" s="1" t="e">
         <v>#N/A</v>
@@ -3540,19 +3541,19 @@
         <v>#N/A</v>
       </c>
       <c r="J56" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="K56" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="L56" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="M56" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="N56" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.35">
@@ -3560,13 +3561,13 @@
         <v>66</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C57" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E57" s="1" t="e">
         <v>#N/A</v>
@@ -3581,19 +3582,19 @@
         <v>#N/A</v>
       </c>
       <c r="J57" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="K57" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="L57" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="M57" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="N57" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="58" spans="1:14" x14ac:dyDescent="0.35">
@@ -3601,10 +3602,10 @@
         <v>67</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E58" s="1" t="e">
         <v>#N/A</v>
@@ -3620,19 +3621,19 @@
       </c>
       <c r="I58"/>
       <c r="J58" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="K58" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="L58" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="M58" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="N58" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="59" spans="1:14" x14ac:dyDescent="0.35">
@@ -3640,13 +3641,13 @@
         <v>68</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E59" s="1" t="e">
         <v>#N/A</v>
@@ -3662,19 +3663,19 @@
       </c>
       <c r="I59"/>
       <c r="J59" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="K59" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="L59" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="M59" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="N59" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="60" spans="1:14" x14ac:dyDescent="0.35">
@@ -3682,13 +3683,13 @@
         <v>69</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E60" s="1" t="e">
         <v>#N/A</v>
@@ -3704,19 +3705,19 @@
       </c>
       <c r="I60"/>
       <c r="J60" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="K60" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="L60" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="M60" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="N60" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="61" spans="1:14" x14ac:dyDescent="0.35">
@@ -3724,13 +3725,13 @@
         <v>70</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C61" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E61" s="1" t="e">
         <v>#N/A</v>
@@ -3746,19 +3747,19 @@
       </c>
       <c r="I61"/>
       <c r="J61" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="K61" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="L61" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="M61" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="N61" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="62" spans="1:14" x14ac:dyDescent="0.35">
@@ -3766,13 +3767,13 @@
         <v>71</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C62" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E62" s="1" t="e">
         <v>#N/A</v>
@@ -3787,19 +3788,19 @@
         <v>#N/A</v>
       </c>
       <c r="J62" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="K62" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="L62" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="M62" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="N62" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="63" spans="1:14" x14ac:dyDescent="0.35">
@@ -3807,13 +3808,13 @@
         <v>72</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C63" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E63" s="1" t="e">
         <v>#N/A</v>
@@ -3828,19 +3829,19 @@
         <v>#N/A</v>
       </c>
       <c r="J63" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="K63" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="L63" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="M63" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="N63" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="64" spans="1:14" x14ac:dyDescent="0.35">
@@ -3848,13 +3849,13 @@
         <v>73</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C64" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E64" s="1" t="e">
         <v>#N/A</v>
@@ -3869,19 +3870,19 @@
         <v>#N/A</v>
       </c>
       <c r="J64" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="K64" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="L64" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="M64" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="N64" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="65" spans="1:14" x14ac:dyDescent="0.35">
@@ -3889,13 +3890,13 @@
         <v>74</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E65" s="1" t="e">
         <v>#N/A</v>
@@ -3910,19 +3911,19 @@
         <v>#N/A</v>
       </c>
       <c r="J65" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="K65" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="L65" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="M65" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="N65" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="66" spans="1:14" x14ac:dyDescent="0.35">
@@ -3930,13 +3931,13 @@
         <v>75</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C66" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E66" s="1" t="e">
         <v>#N/A</v>
@@ -3951,19 +3952,19 @@
         <v>#N/A</v>
       </c>
       <c r="J66" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="K66" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="L66" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="M66" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="N66" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="67" spans="1:14" x14ac:dyDescent="0.35">
@@ -3971,13 +3972,13 @@
         <v>76</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C67" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E67" s="1" t="e">
         <v>#N/A</v>
@@ -3992,19 +3993,19 @@
         <v>#N/A</v>
       </c>
       <c r="J67" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="K67" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="L67" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="M67" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="N67" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="68" spans="1:14" x14ac:dyDescent="0.35">
@@ -4012,13 +4013,13 @@
         <v>77</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C68" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E68" s="1" t="e">
         <v>#N/A</v>
@@ -4033,19 +4034,19 @@
         <v>#N/A</v>
       </c>
       <c r="J68" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="K68" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="L68" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="M68" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="N68" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="69" spans="1:14" x14ac:dyDescent="0.35">
@@ -4053,13 +4054,13 @@
         <v>78</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C69" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E69" s="1" t="e">
         <v>#N/A</v>
@@ -4074,19 +4075,19 @@
         <v>#N/A</v>
       </c>
       <c r="J69" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="K69" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="L69" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="M69" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="N69" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="70" spans="1:14" x14ac:dyDescent="0.35">
@@ -4094,13 +4095,13 @@
         <v>79</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C70" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E70" s="1" t="e">
         <v>#N/A</v>
@@ -4115,19 +4116,19 @@
         <v>#N/A</v>
       </c>
       <c r="J70" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="K70" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="L70" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="M70" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="N70" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="71" spans="1:14" x14ac:dyDescent="0.35">
@@ -4135,13 +4136,13 @@
         <v>80</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C71" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E71" s="1" t="e">
         <v>#N/A</v>
@@ -4156,19 +4157,19 @@
         <v>#N/A</v>
       </c>
       <c r="J71" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="K71" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="L71" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="M71" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="N71" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="72" spans="1:14" x14ac:dyDescent="0.35">
@@ -4176,13 +4177,13 @@
         <v>81</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C72" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E72" s="1" t="e">
         <v>#N/A</v>
@@ -4198,19 +4199,19 @@
       </c>
       <c r="I72"/>
       <c r="J72" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="K72" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="L72" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="M72" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="N72" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="73" spans="1:14" x14ac:dyDescent="0.35">
@@ -4218,13 +4219,13 @@
         <v>82</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C73" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E73" s="1" t="e">
         <v>#N/A</v>
@@ -4239,22 +4240,22 @@
         <v>#N/A</v>
       </c>
       <c r="I73" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="J73" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="K73" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="L73" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="M73" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="N73" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="74" spans="1:14" x14ac:dyDescent="0.35">
@@ -4262,10 +4263,10 @@
         <v>83</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E74" s="1" t="e">
         <v>#N/A</v>
@@ -4280,22 +4281,22 @@
         <v>#N/A</v>
       </c>
       <c r="I74" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="J74" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="K74" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="L74" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="M74" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="N74" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="75" spans="1:14" x14ac:dyDescent="0.35">
@@ -4303,10 +4304,10 @@
         <v>84</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E75" s="1" t="e">
         <v>#N/A</v>
@@ -4321,22 +4322,22 @@
         <v>#N/A</v>
       </c>
       <c r="I75" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="J75" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="K75" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="L75" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="M75" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="N75" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="76" spans="1:14" x14ac:dyDescent="0.35">
@@ -4344,13 +4345,13 @@
         <v>85</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C76" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E76" s="1" t="e">
         <v>#N/A</v>
@@ -4365,22 +4366,22 @@
         <v>#N/A</v>
       </c>
       <c r="I76" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="J76" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="K76" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="L76" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="M76" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="N76" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="77" spans="1:14" x14ac:dyDescent="0.35">
@@ -4388,13 +4389,13 @@
         <v>86</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C77" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E77" s="1" t="e">
         <v>#N/A</v>
@@ -4409,22 +4410,22 @@
         <v>#N/A</v>
       </c>
       <c r="I77" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="J77" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="K77" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="L77" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="M77" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="N77" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="78" spans="1:14" x14ac:dyDescent="0.35">
@@ -4432,13 +4433,13 @@
         <v>87</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C78" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E78" s="1" t="e">
         <v>#N/A</v>
@@ -4453,22 +4454,22 @@
         <v>#N/A</v>
       </c>
       <c r="I78" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="J78" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="K78" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="L78" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="M78" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="N78" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="79" spans="1:14" x14ac:dyDescent="0.35">
@@ -4476,13 +4477,13 @@
         <v>88</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C79" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E79" s="1" t="e">
         <v>#N/A</v>
@@ -4491,51 +4492,51 @@
         <v>#N/A</v>
       </c>
       <c r="G79" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="H79" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="H79" s="1" t="s">
+      <c r="I79" s="1" t="s">
         <v>252</v>
       </c>
-      <c r="I79" s="1" t="s">
-        <v>253</v>
-      </c>
       <c r="J79" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="K79" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="L79" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="M79" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="N79" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="80" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B80" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C80" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="G80" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="H80" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="H80" s="1" t="s">
+      <c r="I80" s="1" t="s">
         <v>252</v>
       </c>
-      <c r="I80" s="1" t="s">
-        <v>253</v>
-      </c>
       <c r="J80" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="81" spans="1:14" x14ac:dyDescent="0.35">
@@ -4543,13 +4544,13 @@
         <v>89</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C81" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E81" s="1" t="e">
         <v>#N/A</v>
@@ -4564,22 +4565,22 @@
         <v>#N/A</v>
       </c>
       <c r="I81" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="J81" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="K81" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="L81" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="M81" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="N81" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="82" spans="1:14" x14ac:dyDescent="0.35">
@@ -4587,13 +4588,13 @@
         <v>90</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C82" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E82" s="1" t="e">
         <v>#N/A</v>
@@ -4602,51 +4603,51 @@
         <v>#N/A</v>
       </c>
       <c r="G82" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="H82" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="H82" s="1" t="s">
+      <c r="I82" s="1" t="s">
         <v>252</v>
       </c>
-      <c r="I82" s="1" t="s">
-        <v>253</v>
-      </c>
       <c r="J82" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="K82" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="L82" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="M82" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="N82" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="83" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B83" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C83" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="G83" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="H83" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="H83" s="1" t="s">
+      <c r="I83" s="1" t="s">
         <v>252</v>
       </c>
-      <c r="I83" s="1" t="s">
-        <v>253</v>
-      </c>
       <c r="J83" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="84" spans="1:14" x14ac:dyDescent="0.35">
@@ -4654,13 +4655,13 @@
         <v>91</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C84" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E84" s="1" t="e">
         <v>#N/A</v>
@@ -4675,22 +4676,22 @@
         <v>#N/A</v>
       </c>
       <c r="I84" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="J84" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="K84" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="L84" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="M84" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="N84" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="85" spans="1:14" x14ac:dyDescent="0.35">
@@ -4698,13 +4699,13 @@
         <v>92</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C85" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E85" s="1" t="e">
         <v>#N/A</v>
@@ -4719,22 +4720,22 @@
         <v>#N/A</v>
       </c>
       <c r="I85" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="J85" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="K85" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="L85" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="M85" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="N85" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="86" spans="1:14" x14ac:dyDescent="0.35">
@@ -4742,13 +4743,13 @@
         <v>93</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C86" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E86" s="1" t="e">
         <v>#N/A</v>
@@ -4763,22 +4764,22 @@
         <v>#N/A</v>
       </c>
       <c r="I86" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="J86" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="K86" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="L86" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="M86" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="N86" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
   </sheetData>

</xml_diff>